<commit_message>
Updates to Radar Sites.xlsx
</commit_message>
<xml_diff>
--- a/Radar Sites.xlsx
+++ b/Radar Sites.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ashwin\Programming\code\VS_8.1\Rad\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f2b5f44ce49b671e/Ashwin/Visual Studio/Rad/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="467">
   <si>
     <t>ON</t>
   </si>
@@ -1327,13 +1327,112 @@
   </si>
   <si>
     <t>Milwaukee</t>
+  </si>
+  <si>
+    <t>NATAK</t>
+  </si>
+  <si>
+    <t>centgrtlakes</t>
+  </si>
+  <si>
+    <t>NATPR</t>
+  </si>
+  <si>
+    <t>northeast</t>
+  </si>
+  <si>
+    <t>northrockies</t>
+  </si>
+  <si>
+    <t>pacnorthwest</t>
+  </si>
+  <si>
+    <t>pacsouthwest</t>
+  </si>
+  <si>
+    <t>southeast</t>
+  </si>
+  <si>
+    <t>southmissvly</t>
+  </si>
+  <si>
+    <t>southplains</t>
+  </si>
+  <si>
+    <t>southrockies</t>
+  </si>
+  <si>
+    <t>uppermissvly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alaska </t>
+  </si>
+  <si>
+    <t>Sector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Central Great Lakes </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hawaii </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northeast </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northern Rockies </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pacific Northwest </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pacific Southwest </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Southeast </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Southern Mississippi Valley </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Southern Plains </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Southern Rockies </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Upper Mississippi Valley </t>
+  </si>
+  <si>
+    <t>Cities</t>
+  </si>
+  <si>
+    <t>Option</t>
+  </si>
+  <si>
+    <t>Base</t>
+  </si>
+  <si>
+    <t>Composite</t>
+  </si>
+  <si>
+    <t>N0R</t>
+  </si>
+  <si>
+    <t>NCR</t>
+  </si>
+  <si>
+    <t>"http://radar.weather.gov/ridge/RadarImg/" + "option/" + "station/" + "station_YYYYMMDD_hhmm_option.gif"</t>
+  </si>
+  <si>
+    <t>“http://radar.weather.gov/Conus/RadarImg/” + "sector/" + "_YYYYMMDD_hhmm.gif"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1344,6 +1443,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF1F497D"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1369,11 +1474,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2054,1708 +2160,1837 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C154"/>
+  <dimension ref="A1:F169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A152" workbookViewId="0">
-      <selection activeCell="A174" sqref="A174"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>355</v>
+        <v>447</v>
       </c>
       <c r="B1" t="s">
-        <v>356</v>
-      </c>
-      <c r="C1" t="s">
-        <v>88</v>
+        <v>466</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>357</v>
-      </c>
-      <c r="B2" t="s">
-        <v>358</v>
-      </c>
-      <c r="C2" t="s">
-        <v>88</v>
+      <c r="A2" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>446</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>87</v>
-      </c>
-      <c r="B3" t="s">
-        <v>366</v>
-      </c>
-      <c r="C3" t="s">
-        <v>88</v>
+      <c r="A3" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>448</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>360</v>
-      </c>
-      <c r="B4" t="s">
-        <v>361</v>
-      </c>
-      <c r="C4" t="s">
-        <v>88</v>
+      <c r="A4" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>449</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B5" t="s">
-        <v>365</v>
-      </c>
-      <c r="C5" t="s">
-        <v>88</v>
+      <c r="A5" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>450</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>362</v>
-      </c>
-      <c r="B6" t="s">
-        <v>363</v>
-      </c>
-      <c r="C6" t="s">
-        <v>88</v>
+      <c r="A6" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>451</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>359</v>
-      </c>
-      <c r="B7" t="s">
-        <v>364</v>
-      </c>
-      <c r="C7" t="s">
-        <v>88</v>
+      <c r="A7" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>452</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>118</v>
-      </c>
-      <c r="B8" t="s">
-        <v>353</v>
-      </c>
-      <c r="C8" t="s">
-        <v>119</v>
+      <c r="A8" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>295</v>
-      </c>
-      <c r="B9" t="s">
-        <v>367</v>
-      </c>
-      <c r="C9" t="s">
-        <v>119</v>
+      <c r="A9" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>176</v>
-      </c>
-      <c r="B10" t="s">
-        <v>354</v>
-      </c>
-      <c r="C10" t="s">
-        <v>119</v>
+      <c r="A10" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>455</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>227</v>
-      </c>
-      <c r="B11" t="s">
-        <v>368</v>
-      </c>
-      <c r="C11" t="s">
-        <v>119</v>
+      <c r="A11" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>456</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>286</v>
-      </c>
-      <c r="B12" t="s">
-        <v>287</v>
-      </c>
-      <c r="C12" t="s">
-        <v>119</v>
+      <c r="A12" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>272</v>
-      </c>
-      <c r="B13" t="s">
-        <v>273</v>
-      </c>
-      <c r="C13" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>332</v>
-      </c>
-      <c r="B14" t="s">
-        <v>369</v>
-      </c>
-      <c r="C14" t="s">
-        <v>274</v>
+      <c r="A13" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>195</v>
+      <c r="A15" s="2" t="s">
+        <v>459</v>
       </c>
       <c r="B15" t="s">
-        <v>196</v>
-      </c>
-      <c r="C15" t="s">
-        <v>174</v>
+        <v>465</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>355</v>
+      </c>
+      <c r="B16" t="s">
+        <v>356</v>
+      </c>
+      <c r="C16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>357</v>
+      </c>
+      <c r="B17" t="s">
+        <v>358</v>
+      </c>
+      <c r="C17" t="s">
+        <v>88</v>
+      </c>
+      <c r="E17" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>87</v>
+      </c>
+      <c r="B18" t="s">
+        <v>366</v>
+      </c>
+      <c r="C18" t="s">
+        <v>88</v>
+      </c>
+      <c r="E18" t="s">
+        <v>461</v>
+      </c>
+      <c r="F18" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>360</v>
+      </c>
+      <c r="B19" t="s">
+        <v>361</v>
+      </c>
+      <c r="C19" t="s">
+        <v>88</v>
+      </c>
+      <c r="E19" t="s">
+        <v>462</v>
+      </c>
+      <c r="F19" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>89</v>
+      </c>
+      <c r="B20" t="s">
+        <v>365</v>
+      </c>
+      <c r="C20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>362</v>
+      </c>
+      <c r="B21" t="s">
+        <v>363</v>
+      </c>
+      <c r="C21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>359</v>
+      </c>
+      <c r="B22" t="s">
+        <v>364</v>
+      </c>
+      <c r="C22" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>118</v>
+      </c>
+      <c r="B23" t="s">
+        <v>353</v>
+      </c>
+      <c r="C23" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>295</v>
+      </c>
+      <c r="B24" t="s">
+        <v>367</v>
+      </c>
+      <c r="C24" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>176</v>
+      </c>
+      <c r="B25" t="s">
+        <v>354</v>
+      </c>
+      <c r="C25" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>227</v>
+      </c>
+      <c r="B26" t="s">
+        <v>368</v>
+      </c>
+      <c r="C26" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>286</v>
+      </c>
+      <c r="B27" t="s">
+        <v>287</v>
+      </c>
+      <c r="C27" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>272</v>
+      </c>
+      <c r="B28" t="s">
+        <v>273</v>
+      </c>
+      <c r="C28" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>332</v>
+      </c>
+      <c r="B29" t="s">
+        <v>369</v>
+      </c>
+      <c r="C29" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>195</v>
+      </c>
+      <c r="B30" t="s">
+        <v>196</v>
+      </c>
+      <c r="C30" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>241</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B31" t="s">
         <v>370</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C31" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>172</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B32" t="s">
         <v>173</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C32" t="s">
         <v>174</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>351</v>
-      </c>
-      <c r="B18" t="s">
-        <v>352</v>
-      </c>
-      <c r="C18" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>104</v>
-      </c>
-      <c r="B19" t="s">
-        <v>105</v>
-      </c>
-      <c r="C19" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>184</v>
-      </c>
-      <c r="B20" t="s">
-        <v>185</v>
-      </c>
-      <c r="C20" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>111</v>
-      </c>
-      <c r="B21" t="s">
-        <v>110</v>
-      </c>
-      <c r="C21" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>350</v>
-      </c>
-      <c r="B22" t="s">
-        <v>375</v>
-      </c>
-      <c r="C22" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>151</v>
-      </c>
-      <c r="B23" t="s">
-        <v>372</v>
-      </c>
-      <c r="C23" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>298</v>
-      </c>
-      <c r="B24" t="s">
-        <v>299</v>
-      </c>
-      <c r="C24" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>296</v>
-      </c>
-      <c r="B25" t="s">
-        <v>373</v>
-      </c>
-      <c r="C25" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>224</v>
-      </c>
-      <c r="B26" t="s">
-        <v>371</v>
-      </c>
-      <c r="C26" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>331</v>
-      </c>
-      <c r="B27" t="s">
-        <v>374</v>
-      </c>
-      <c r="C27" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>346</v>
-      </c>
-      <c r="B28" t="s">
-        <v>347</v>
-      </c>
-      <c r="C28" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>197</v>
-      </c>
-      <c r="B29" t="s">
-        <v>376</v>
-      </c>
-      <c r="C29" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>202</v>
-      </c>
-      <c r="B30" t="s">
-        <v>203</v>
-      </c>
-      <c r="C30" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>313</v>
-      </c>
-      <c r="B31" t="s">
-        <v>314</v>
-      </c>
-      <c r="C31" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>164</v>
-      </c>
-      <c r="B32" t="s">
-        <v>165</v>
-      </c>
-      <c r="C32" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>243</v>
+        <v>351</v>
       </c>
       <c r="B33" t="s">
-        <v>244</v>
+        <v>352</v>
       </c>
       <c r="C33" t="s">
-        <v>97</v>
+        <v>174</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
       <c r="B34" t="s">
-        <v>127</v>
+        <v>105</v>
       </c>
       <c r="C34" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>284</v>
+        <v>184</v>
       </c>
       <c r="B35" t="s">
-        <v>285</v>
+        <v>185</v>
       </c>
       <c r="C35" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="B36" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="C36" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>182</v>
+        <v>350</v>
       </c>
       <c r="B37" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="C37" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>336</v>
+        <v>151</v>
       </c>
       <c r="B38" t="s">
-        <v>337</v>
+        <v>372</v>
       </c>
       <c r="C38" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>333</v>
+        <v>298</v>
       </c>
       <c r="B39" t="s">
-        <v>379</v>
+        <v>299</v>
       </c>
       <c r="C39" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>191</v>
+        <v>296</v>
       </c>
       <c r="B40" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
       <c r="C40" t="s">
-        <v>192</v>
+        <v>106</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>344</v>
+        <v>224</v>
       </c>
       <c r="B41" t="s">
-        <v>345</v>
+        <v>371</v>
       </c>
       <c r="C41" t="s">
-        <v>192</v>
+        <v>106</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>245</v>
+        <v>331</v>
       </c>
       <c r="B42" t="s">
-        <v>246</v>
+        <v>374</v>
       </c>
       <c r="C42" t="s">
-        <v>192</v>
+        <v>106</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>218</v>
+        <v>346</v>
       </c>
       <c r="B43" t="s">
-        <v>382</v>
+        <v>347</v>
       </c>
       <c r="C43" t="s">
-        <v>219</v>
+        <v>106</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>220</v>
+        <v>197</v>
       </c>
       <c r="B44" t="s">
-        <v>221</v>
+        <v>376</v>
       </c>
       <c r="C44" t="s">
-        <v>219</v>
+        <v>198</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
       <c r="B45" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="C45" t="s">
-        <v>219</v>
+        <v>198</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>228</v>
+        <v>313</v>
       </c>
       <c r="B46" t="s">
-        <v>381</v>
+        <v>314</v>
       </c>
       <c r="C46" t="s">
-        <v>219</v>
+        <v>198</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B47" t="s">
-        <v>383</v>
+        <v>165</v>
       </c>
       <c r="C47" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>168</v>
+        <v>243</v>
       </c>
       <c r="B48" t="s">
-        <v>384</v>
+        <v>244</v>
       </c>
       <c r="C48" t="s">
-        <v>163</v>
+        <v>97</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="B49" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="C49" t="s">
-        <v>135</v>
+        <v>97</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>323</v>
+        <v>284</v>
       </c>
       <c r="B50" t="s">
-        <v>324</v>
+        <v>285</v>
       </c>
       <c r="C50" t="s">
-        <v>135</v>
+        <v>97</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>235</v>
+        <v>95</v>
       </c>
       <c r="B51" t="s">
-        <v>385</v>
+        <v>96</v>
       </c>
       <c r="C51" t="s">
-        <v>236</v>
+        <v>97</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>262</v>
+        <v>182</v>
       </c>
       <c r="B52" t="s">
-        <v>263</v>
+        <v>378</v>
       </c>
       <c r="C52" t="s">
-        <v>236</v>
+        <v>97</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>237</v>
+        <v>336</v>
       </c>
       <c r="B53" t="s">
-        <v>238</v>
+        <v>337</v>
       </c>
       <c r="C53" t="s">
-        <v>239</v>
+        <v>97</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>242</v>
+        <v>333</v>
       </c>
       <c r="B54" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="C54" t="s">
-        <v>239</v>
+        <v>97</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>152</v>
+        <v>191</v>
       </c>
       <c r="B55" t="s">
-        <v>153</v>
+        <v>380</v>
       </c>
       <c r="C55" t="s">
-        <v>154</v>
+        <v>192</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>204</v>
+        <v>344</v>
       </c>
       <c r="B56" t="s">
-        <v>205</v>
+        <v>345</v>
       </c>
       <c r="C56" t="s">
-        <v>154</v>
+        <v>192</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>339</v>
+        <v>245</v>
       </c>
       <c r="B57" t="s">
-        <v>387</v>
+        <v>246</v>
       </c>
       <c r="C57" t="s">
-        <v>154</v>
+        <v>192</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="B58" t="s">
-        <v>230</v>
+        <v>382</v>
       </c>
       <c r="C58" t="s">
-        <v>154</v>
+        <v>219</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="B59" t="s">
-        <v>388</v>
+        <v>221</v>
       </c>
       <c r="C59" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>247</v>
+        <v>222</v>
       </c>
       <c r="B60" t="s">
-        <v>248</v>
+        <v>223</v>
       </c>
       <c r="C60" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>270</v>
+        <v>228</v>
       </c>
       <c r="B61" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="C61" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>307</v>
+        <v>162</v>
       </c>
       <c r="B62" t="s">
-        <v>308</v>
+        <v>383</v>
       </c>
       <c r="C62" t="s">
-        <v>226</v>
+        <v>163</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>312</v>
+        <v>168</v>
       </c>
       <c r="B63" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="C63" t="s">
-        <v>255</v>
+        <v>163</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>253</v>
+        <v>133</v>
       </c>
       <c r="B64" t="s">
-        <v>254</v>
+        <v>134</v>
       </c>
       <c r="C64" t="s">
-        <v>255</v>
+        <v>135</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>256</v>
+        <v>323</v>
       </c>
       <c r="B65" t="s">
-        <v>391</v>
+        <v>324</v>
       </c>
       <c r="C65" t="s">
-        <v>255</v>
+        <v>135</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>327</v>
+        <v>235</v>
       </c>
       <c r="B66" t="s">
-        <v>328</v>
+        <v>385</v>
       </c>
       <c r="C66" t="s">
-        <v>255</v>
+        <v>236</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>120</v>
+        <v>262</v>
       </c>
       <c r="B67" t="s">
-        <v>392</v>
+        <v>263</v>
       </c>
       <c r="C67" t="s">
-        <v>121</v>
+        <v>236</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>131</v>
+        <v>237</v>
       </c>
       <c r="B68" t="s">
-        <v>393</v>
+        <v>238</v>
       </c>
       <c r="C68" t="s">
-        <v>132</v>
+        <v>239</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>214</v>
+        <v>242</v>
       </c>
       <c r="B69" t="s">
-        <v>322</v>
+        <v>386</v>
       </c>
       <c r="C69" t="s">
-        <v>132</v>
+        <v>239</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
       <c r="B70" t="s">
-        <v>395</v>
+        <v>153</v>
       </c>
       <c r="C70" t="s">
-        <v>99</v>
+        <v>154</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>98</v>
+        <v>204</v>
       </c>
       <c r="B71" t="s">
-        <v>394</v>
+        <v>205</v>
       </c>
       <c r="C71" t="s">
-        <v>99</v>
+        <v>154</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>209</v>
+        <v>339</v>
       </c>
       <c r="B72" t="s">
-        <v>210</v>
+        <v>387</v>
       </c>
       <c r="C72" t="s">
-        <v>99</v>
+        <v>154</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>289</v>
+        <v>229</v>
       </c>
       <c r="B73" t="s">
-        <v>290</v>
+        <v>230</v>
       </c>
       <c r="C73" t="s">
-        <v>99</v>
+        <v>154</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>159</v>
+        <v>225</v>
       </c>
       <c r="B74" t="s">
-        <v>160</v>
+        <v>388</v>
       </c>
       <c r="C74" t="s">
-        <v>161</v>
+        <v>226</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>288</v>
+        <v>247</v>
       </c>
       <c r="B75" t="s">
-        <v>396</v>
+        <v>248</v>
       </c>
       <c r="C75" t="s">
-        <v>161</v>
+        <v>226</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>170</v>
+        <v>270</v>
       </c>
       <c r="B76" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="C76" t="s">
-        <v>171</v>
+        <v>226</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>325</v>
+        <v>307</v>
       </c>
       <c r="B77" t="s">
-        <v>326</v>
+        <v>308</v>
       </c>
       <c r="C77" t="s">
-        <v>171</v>
+        <v>226</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>266</v>
+        <v>312</v>
       </c>
       <c r="B78" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="C78" t="s">
-        <v>171</v>
+        <v>255</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>156</v>
+        <v>253</v>
       </c>
       <c r="B79" t="s">
-        <v>399</v>
+        <v>254</v>
       </c>
       <c r="C79" t="s">
-        <v>157</v>
+        <v>255</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>212</v>
+        <v>256</v>
       </c>
       <c r="B80" t="s">
-        <v>213</v>
+        <v>391</v>
       </c>
       <c r="C80" t="s">
-        <v>157</v>
+        <v>255</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>115</v>
+        <v>327</v>
       </c>
       <c r="B81" t="s">
-        <v>116</v>
+        <v>328</v>
       </c>
       <c r="C81" t="s">
-        <v>117</v>
+        <v>255</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>200</v>
+        <v>120</v>
       </c>
       <c r="B82" t="s">
-        <v>201</v>
+        <v>392</v>
       </c>
       <c r="C82" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>334</v>
+        <v>131</v>
       </c>
       <c r="B83" t="s">
-        <v>335</v>
+        <v>393</v>
       </c>
       <c r="C83" t="s">
-        <v>117</v>
+        <v>132</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>293</v>
+        <v>214</v>
       </c>
       <c r="B84" t="s">
-        <v>400</v>
+        <v>322</v>
       </c>
       <c r="C84" t="s">
-        <v>117</v>
+        <v>132</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>282</v>
+        <v>167</v>
       </c>
       <c r="B85" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="C85" t="s">
-        <v>269</v>
+        <v>99</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>315</v>
+        <v>98</v>
       </c>
       <c r="B86" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
       <c r="C86" t="s">
-        <v>269</v>
+        <v>99</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>267</v>
+        <v>209</v>
       </c>
       <c r="B87" t="s">
-        <v>268</v>
+        <v>210</v>
       </c>
       <c r="C87" t="s">
-        <v>269</v>
+        <v>99</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>112</v>
+        <v>289</v>
       </c>
       <c r="B88" t="s">
-        <v>113</v>
+        <v>290</v>
       </c>
       <c r="C88" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>297</v>
+        <v>159</v>
       </c>
       <c r="B89" t="s">
-        <v>403</v>
+        <v>160</v>
       </c>
       <c r="C89" t="s">
-        <v>114</v>
+        <v>161</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>280</v>
+        <v>288</v>
       </c>
       <c r="B90" t="s">
-        <v>281</v>
+        <v>396</v>
       </c>
       <c r="C90" t="s">
-        <v>114</v>
+        <v>161</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>343</v>
+        <v>170</v>
       </c>
       <c r="B91" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
       <c r="C91" t="s">
-        <v>261</v>
+        <v>171</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>259</v>
+        <v>325</v>
       </c>
       <c r="B92" t="s">
-        <v>260</v>
+        <v>326</v>
       </c>
       <c r="C92" t="s">
-        <v>261</v>
+        <v>171</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>301</v>
+        <v>266</v>
       </c>
       <c r="B93" t="s">
-        <v>302</v>
+        <v>398</v>
       </c>
       <c r="C93" t="s">
-        <v>261</v>
+        <v>171</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B94" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="C94" t="s">
-        <v>406</v>
+        <v>157</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>84</v>
+        <v>212</v>
       </c>
       <c r="B95" t="s">
-        <v>85</v>
+        <v>213</v>
       </c>
       <c r="C95" t="s">
-        <v>86</v>
+        <v>157</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>190</v>
+        <v>115</v>
       </c>
       <c r="B96" t="s">
-        <v>407</v>
+        <v>116</v>
       </c>
       <c r="C96" t="s">
-        <v>86</v>
+        <v>117</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="B97" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
       <c r="C97" t="s">
-        <v>86</v>
+        <v>117</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>264</v>
+        <v>334</v>
       </c>
       <c r="B98" t="s">
-        <v>265</v>
+        <v>335</v>
       </c>
       <c r="C98" t="s">
-        <v>181</v>
+        <v>117</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>179</v>
+        <v>293</v>
       </c>
       <c r="B99" t="s">
-        <v>180</v>
+        <v>400</v>
       </c>
       <c r="C99" t="s">
-        <v>181</v>
+        <v>117</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>318</v>
+        <v>282</v>
       </c>
       <c r="B100" t="s">
-        <v>408</v>
+        <v>401</v>
       </c>
       <c r="C100" t="s">
-        <v>181</v>
+        <v>269</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>175</v>
+        <v>315</v>
       </c>
       <c r="B101" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
       <c r="C101" t="s">
-        <v>109</v>
+        <v>269</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>107</v>
+        <v>267</v>
       </c>
       <c r="B102" t="s">
-        <v>108</v>
+        <v>268</v>
       </c>
       <c r="C102" t="s">
-        <v>109</v>
+        <v>269</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="B103" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="C103" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>340</v>
+        <v>297</v>
       </c>
       <c r="B104" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
       <c r="C104" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>304</v>
+        <v>280</v>
       </c>
       <c r="B105" t="s">
-        <v>409</v>
+        <v>281</v>
       </c>
       <c r="C105" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>138</v>
+        <v>343</v>
       </c>
       <c r="B106" t="s">
-        <v>139</v>
+        <v>404</v>
       </c>
       <c r="C106" t="s">
-        <v>140</v>
+        <v>261</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>234</v>
+        <v>259</v>
       </c>
       <c r="B107" t="s">
-        <v>412</v>
+        <v>260</v>
       </c>
       <c r="C107" t="s">
-        <v>140</v>
+        <v>261</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>187</v>
+        <v>301</v>
       </c>
       <c r="B108" t="s">
-        <v>188</v>
+        <v>302</v>
       </c>
       <c r="C108" t="s">
-        <v>189</v>
+        <v>261</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>338</v>
+        <v>158</v>
       </c>
       <c r="B109" t="s">
-        <v>414</v>
+        <v>405</v>
       </c>
       <c r="C109" t="s">
-        <v>189</v>
+        <v>406</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>240</v>
+        <v>84</v>
       </c>
       <c r="B110" t="s">
-        <v>413</v>
+        <v>85</v>
       </c>
       <c r="C110" t="s">
-        <v>189</v>
+        <v>86</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>348</v>
+        <v>190</v>
       </c>
       <c r="B111" t="s">
-        <v>349</v>
+        <v>407</v>
       </c>
       <c r="C111" t="s">
-        <v>189</v>
+        <v>86</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>277</v>
+        <v>215</v>
       </c>
       <c r="B112" t="s">
-        <v>278</v>
+        <v>216</v>
       </c>
       <c r="C112" t="s">
-        <v>279</v>
+        <v>86</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>310</v>
+        <v>264</v>
       </c>
       <c r="B113" t="s">
-        <v>311</v>
+        <v>265</v>
       </c>
       <c r="C113" t="s">
-        <v>279</v>
+        <v>181</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>321</v>
+        <v>179</v>
       </c>
       <c r="B114" t="s">
-        <v>322</v>
+        <v>180</v>
       </c>
       <c r="C114" t="s">
-        <v>279</v>
+        <v>181</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>309</v>
+        <v>318</v>
       </c>
       <c r="B115" t="s">
-        <v>415</v>
+        <v>408</v>
       </c>
       <c r="C115" t="s">
-        <v>137</v>
+        <v>181</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>136</v>
+        <v>175</v>
       </c>
       <c r="B116" t="s">
-        <v>416</v>
+        <v>410</v>
       </c>
       <c r="C116" t="s">
-        <v>137</v>
+        <v>109</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>249</v>
+        <v>107</v>
       </c>
       <c r="B117" t="s">
-        <v>417</v>
+        <v>108</v>
       </c>
       <c r="C117" t="s">
-        <v>250</v>
+        <v>109</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="B118" t="s">
-        <v>142</v>
+        <v>125</v>
       </c>
       <c r="C118" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>128</v>
+        <v>340</v>
       </c>
       <c r="B119" t="s">
-        <v>129</v>
+        <v>411</v>
       </c>
       <c r="C119" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>211</v>
+        <v>304</v>
       </c>
       <c r="B120" t="s">
-        <v>418</v>
+        <v>409</v>
       </c>
       <c r="C120" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>81</v>
+        <v>138</v>
       </c>
       <c r="B121" t="s">
-        <v>82</v>
+        <v>139</v>
       </c>
       <c r="C121" t="s">
-        <v>83</v>
+        <v>140</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>341</v>
+        <v>234</v>
       </c>
       <c r="B122" t="s">
-        <v>342</v>
+        <v>412</v>
       </c>
       <c r="C122" t="s">
-        <v>83</v>
+        <v>140</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="B123" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="C123" t="s">
-        <v>83</v>
+        <v>189</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>291</v>
+        <v>338</v>
       </c>
       <c r="B124" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="C124" t="s">
-        <v>292</v>
+        <v>189</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>300</v>
+        <v>240</v>
       </c>
       <c r="B125" t="s">
-        <v>420</v>
+        <v>413</v>
       </c>
       <c r="C125" t="s">
-        <v>292</v>
+        <v>189</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>303</v>
+        <v>348</v>
       </c>
       <c r="B126" t="s">
-        <v>421</v>
+        <v>349</v>
       </c>
       <c r="C126" t="s">
-        <v>292</v>
+        <v>189</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>92</v>
+        <v>277</v>
       </c>
       <c r="B127" t="s">
-        <v>93</v>
+        <v>278</v>
       </c>
       <c r="C127" t="s">
-        <v>94</v>
+        <v>279</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>183</v>
+        <v>310</v>
       </c>
       <c r="B128" t="s">
-        <v>426</v>
+        <v>311</v>
       </c>
       <c r="C128" t="s">
-        <v>94</v>
+        <v>279</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>122</v>
+        <v>321</v>
       </c>
       <c r="B129" t="s">
-        <v>123</v>
+        <v>322</v>
       </c>
       <c r="C129" t="s">
-        <v>94</v>
+        <v>279</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>208</v>
+        <v>309</v>
       </c>
       <c r="B130" t="s">
-        <v>423</v>
+        <v>415</v>
       </c>
       <c r="C130" t="s">
-        <v>94</v>
+        <v>137</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B131" t="s">
-        <v>144</v>
+        <v>416</v>
       </c>
       <c r="C131" t="s">
-        <v>94</v>
+        <v>137</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>199</v>
+        <v>249</v>
       </c>
       <c r="B132" t="s">
-        <v>427</v>
+        <v>417</v>
       </c>
       <c r="C132" t="s">
-        <v>94</v>
+        <v>250</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>169</v>
+        <v>141</v>
       </c>
       <c r="B133" t="s">
-        <v>425</v>
+        <v>142</v>
       </c>
       <c r="C133" t="s">
-        <v>94</v>
+        <v>130</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>177</v>
+        <v>128</v>
       </c>
       <c r="B134" t="s">
-        <v>178</v>
+        <v>129</v>
       </c>
       <c r="C134" t="s">
-        <v>94</v>
+        <v>130</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="B135" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="C135" t="s">
-        <v>94</v>
+        <v>130</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>155</v>
+        <v>81</v>
       </c>
       <c r="B136" t="s">
-        <v>422</v>
+        <v>82</v>
       </c>
       <c r="C136" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>251</v>
+        <v>341</v>
       </c>
       <c r="B137" t="s">
-        <v>252</v>
+        <v>342</v>
       </c>
       <c r="C137" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>275</v>
+        <v>193</v>
       </c>
       <c r="B138" t="s">
-        <v>276</v>
+        <v>194</v>
       </c>
       <c r="C138" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>329</v>
+        <v>291</v>
       </c>
       <c r="B139" t="s">
-        <v>330</v>
+        <v>419</v>
       </c>
       <c r="C139" t="s">
-        <v>94</v>
+        <v>292</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>231</v>
+        <v>300</v>
       </c>
       <c r="B140" t="s">
-        <v>232</v>
+        <v>420</v>
       </c>
       <c r="C140" t="s">
-        <v>233</v>
+        <v>292</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>294</v>
+        <v>303</v>
       </c>
       <c r="B141" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="C141" t="s">
-        <v>233</v>
+        <v>292</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>186</v>
+        <v>92</v>
       </c>
       <c r="B142" t="s">
-        <v>429</v>
+        <v>93</v>
       </c>
       <c r="C142" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>271</v>
+        <v>183</v>
       </c>
       <c r="B143" t="s">
-        <v>377</v>
+        <v>426</v>
       </c>
       <c r="C143" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>90</v>
+        <v>122</v>
       </c>
       <c r="B144" t="s">
-        <v>430</v>
+        <v>123</v>
       </c>
       <c r="C144" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>145</v>
+        <v>208</v>
       </c>
       <c r="B145" t="s">
-        <v>146</v>
+        <v>423</v>
       </c>
       <c r="C145" t="s">
-        <v>147</v>
+        <v>94</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>257</v>
+        <v>143</v>
       </c>
       <c r="B146" t="s">
-        <v>258</v>
+        <v>144</v>
       </c>
       <c r="C146" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>102</v>
+        <v>199</v>
       </c>
       <c r="B147" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="C147" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>305</v>
+        <v>169</v>
       </c>
       <c r="B148" t="s">
-        <v>306</v>
+        <v>425</v>
       </c>
       <c r="C148" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>206</v>
+        <v>177</v>
       </c>
       <c r="B149" t="s">
-        <v>207</v>
+        <v>178</v>
       </c>
       <c r="C149" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>100</v>
+        <v>217</v>
       </c>
       <c r="B150" t="s">
-        <v>432</v>
+        <v>424</v>
       </c>
       <c r="C150" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>283</v>
+        <v>155</v>
       </c>
       <c r="B151" t="s">
-        <v>433</v>
+        <v>422</v>
       </c>
       <c r="C151" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>319</v>
+        <v>251</v>
       </c>
       <c r="B152" t="s">
-        <v>142</v>
+        <v>252</v>
       </c>
       <c r="C152" t="s">
-        <v>320</v>
+        <v>94</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>148</v>
+        <v>275</v>
       </c>
       <c r="B153" t="s">
-        <v>149</v>
+        <v>276</v>
       </c>
       <c r="C153" t="s">
-        <v>150</v>
+        <v>94</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
+        <v>329</v>
+      </c>
+      <c r="B154" t="s">
+        <v>330</v>
+      </c>
+      <c r="C154" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>231</v>
+      </c>
+      <c r="B155" t="s">
+        <v>232</v>
+      </c>
+      <c r="C155" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>294</v>
+      </c>
+      <c r="B156" t="s">
+        <v>428</v>
+      </c>
+      <c r="C156" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>186</v>
+      </c>
+      <c r="B157" t="s">
+        <v>429</v>
+      </c>
+      <c r="C157" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>271</v>
+      </c>
+      <c r="B158" t="s">
+        <v>377</v>
+      </c>
+      <c r="C158" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>90</v>
+      </c>
+      <c r="B159" t="s">
+        <v>430</v>
+      </c>
+      <c r="C159" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>145</v>
+      </c>
+      <c r="B160" t="s">
+        <v>146</v>
+      </c>
+      <c r="C160" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>257</v>
+      </c>
+      <c r="B161" t="s">
+        <v>258</v>
+      </c>
+      <c r="C161" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>102</v>
+      </c>
+      <c r="B162" t="s">
+        <v>431</v>
+      </c>
+      <c r="C162" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>305</v>
+      </c>
+      <c r="B163" t="s">
+        <v>306</v>
+      </c>
+      <c r="C163" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>206</v>
+      </c>
+      <c r="B164" t="s">
+        <v>207</v>
+      </c>
+      <c r="C164" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>100</v>
+      </c>
+      <c r="B165" t="s">
+        <v>432</v>
+      </c>
+      <c r="C165" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>283</v>
+      </c>
+      <c r="B166" t="s">
+        <v>433</v>
+      </c>
+      <c r="C166" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>319</v>
+      </c>
+      <c r="B167" t="s">
+        <v>142</v>
+      </c>
+      <c r="C167" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>148</v>
+      </c>
+      <c r="B168" t="s">
+        <v>149</v>
+      </c>
+      <c r="C168" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
         <v>316</v>
       </c>
-      <c r="B154" t="s">
+      <c r="B169" t="s">
         <v>317</v>
       </c>
-      <c r="C154" t="s">
+      <c r="C169" t="s">
         <v>150</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added new US data to XML
1. Added XML files for US data
2.  Added code to read province names from XML files
</commit_message>
<xml_diff>
--- a/Radar Sites.xlsx
+++ b/Radar Sites.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="490">
   <si>
     <t>ON</t>
   </si>
@@ -1327,6 +1327,174 @@
   </si>
   <si>
     <t>Milwaukee</t>
+  </si>
+  <si>
+    <t>Alabama</t>
+  </si>
+  <si>
+    <t>Alaska</t>
+  </si>
+  <si>
+    <t>Arizona</t>
+  </si>
+  <si>
+    <t>Arkansas</t>
+  </si>
+  <si>
+    <t>California</t>
+  </si>
+  <si>
+    <t>Colorado</t>
+  </si>
+  <si>
+    <t>Connecticut</t>
+  </si>
+  <si>
+    <t>CT</t>
+  </si>
+  <si>
+    <t>Delaware</t>
+  </si>
+  <si>
+    <t>Florida</t>
+  </si>
+  <si>
+    <t>Georgia</t>
+  </si>
+  <si>
+    <t>Hawaii</t>
+  </si>
+  <si>
+    <t>Idaho</t>
+  </si>
+  <si>
+    <t>Illinois</t>
+  </si>
+  <si>
+    <t>Indiana</t>
+  </si>
+  <si>
+    <t>Iowa</t>
+  </si>
+  <si>
+    <t>Kansas</t>
+  </si>
+  <si>
+    <t>Kentucky</t>
+  </si>
+  <si>
+    <t>Louisiana</t>
+  </si>
+  <si>
+    <t>Maine</t>
+  </si>
+  <si>
+    <t>Maryland</t>
+  </si>
+  <si>
+    <t>MD</t>
+  </si>
+  <si>
+    <t>Massachusetts</t>
+  </si>
+  <si>
+    <t>Michigan</t>
+  </si>
+  <si>
+    <t>Minnesota</t>
+  </si>
+  <si>
+    <t>Mississippi</t>
+  </si>
+  <si>
+    <t>Missouri</t>
+  </si>
+  <si>
+    <t>Montana</t>
+  </si>
+  <si>
+    <t>Nebraska</t>
+  </si>
+  <si>
+    <t>Nevada</t>
+  </si>
+  <si>
+    <t>New Hampshire</t>
+  </si>
+  <si>
+    <t>NH</t>
+  </si>
+  <si>
+    <t>New Jersey</t>
+  </si>
+  <si>
+    <t>New Mexico</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>North Carolina</t>
+  </si>
+  <si>
+    <t>North Dakota</t>
+  </si>
+  <si>
+    <t>Ohio</t>
+  </si>
+  <si>
+    <t>Oklahoma</t>
+  </si>
+  <si>
+    <t>Oregon</t>
+  </si>
+  <si>
+    <t>Pennsylvania</t>
+  </si>
+  <si>
+    <t>Rhode Island</t>
+  </si>
+  <si>
+    <t>RI</t>
+  </si>
+  <si>
+    <t>South Carolina</t>
+  </si>
+  <si>
+    <t>South Dakota</t>
+  </si>
+  <si>
+    <t>Tennessee</t>
+  </si>
+  <si>
+    <t>Texas</t>
+  </si>
+  <si>
+    <t>Utah</t>
+  </si>
+  <si>
+    <t>Vermont</t>
+  </si>
+  <si>
+    <t>Virginia</t>
+  </si>
+  <si>
+    <t>Washington</t>
+  </si>
+  <si>
+    <t>West Virginia</t>
+  </si>
+  <si>
+    <t>Wisconsin</t>
+  </si>
+  <si>
+    <t>Wyoming</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Code</t>
   </si>
 </sst>
 </file>
@@ -1369,10 +1537,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2054,10 +2225,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C154"/>
+  <dimension ref="A1:L154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A152" workbookViewId="0">
-      <selection activeCell="A174" sqref="A174"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2065,7 +2236,7 @@
     <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>355</v>
       </c>
@@ -2075,8 +2246,18 @@
       <c r="C1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="str">
+        <f>INDEX(I$2:I$51,MATCH(C1,J$2:J$51,0))</f>
+        <v>Alaska</v>
+      </c>
+      <c r="I1" t="s">
+        <v>488</v>
+      </c>
+      <c r="J1" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>357</v>
       </c>
@@ -2086,8 +2267,18 @@
       <c r="C2" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="str">
+        <f t="shared" ref="D2:D65" si="0">INDEX(I$2:I$51,MATCH(C2,J$2:J$51,0))</f>
+        <v>Alaska</v>
+      </c>
+      <c r="I2" t="s">
+        <v>434</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>87</v>
       </c>
@@ -2097,8 +2288,18 @@
       <c r="C3" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="str">
+        <f t="shared" si="0"/>
+        <v>Alaska</v>
+      </c>
+      <c r="I3" t="s">
+        <v>435</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>360</v>
       </c>
@@ -2108,8 +2309,26 @@
       <c r="C4" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>Alaska</v>
+      </c>
+      <c r="I4" t="s">
+        <v>436</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="K4">
+        <f>MATCH(C1,J2:J51,)</f>
+        <v>2</v>
+      </c>
+      <c r="L4" t="str">
+        <f>INDEX(I2:I51,2)</f>
+        <v>Alaska</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>89</v>
       </c>
@@ -2119,8 +2338,18 @@
       <c r="C5" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>Alaska</v>
+      </c>
+      <c r="I5" t="s">
+        <v>437</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>362</v>
       </c>
@@ -2130,8 +2359,18 @@
       <c r="C6" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>Alaska</v>
+      </c>
+      <c r="I6" t="s">
+        <v>438</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>359</v>
       </c>
@@ -2141,8 +2380,18 @@
       <c r="C7" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>Alaska</v>
+      </c>
+      <c r="I7" t="s">
+        <v>439</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>118</v>
       </c>
@@ -2152,8 +2401,18 @@
       <c r="C8" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>Alabama</v>
+      </c>
+      <c r="I8" t="s">
+        <v>440</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>295</v>
       </c>
@@ -2163,8 +2422,18 @@
       <c r="C9" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>Alabama</v>
+      </c>
+      <c r="I9" t="s">
+        <v>442</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>176</v>
       </c>
@@ -2174,8 +2443,18 @@
       <c r="C10" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>Alabama</v>
+      </c>
+      <c r="I10" t="s">
+        <v>443</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>227</v>
       </c>
@@ -2185,8 +2464,18 @@
       <c r="C11" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>Alabama</v>
+      </c>
+      <c r="I11" t="s">
+        <v>444</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>286</v>
       </c>
@@ -2196,8 +2485,18 @@
       <c r="C12" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>Alabama</v>
+      </c>
+      <c r="I12" t="s">
+        <v>445</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>272</v>
       </c>
@@ -2207,8 +2506,18 @@
       <c r="C13" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>Arkansas</v>
+      </c>
+      <c r="I13" t="s">
+        <v>446</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>332</v>
       </c>
@@ -2218,8 +2527,18 @@
       <c r="C14" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v>Arkansas</v>
+      </c>
+      <c r="I14" t="s">
+        <v>447</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>195</v>
       </c>
@@ -2229,8 +2548,18 @@
       <c r="C15" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v>Arizona</v>
+      </c>
+      <c r="I15" t="s">
+        <v>448</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>241</v>
       </c>
@@ -2240,8 +2569,18 @@
       <c r="C16" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v>Arizona</v>
+      </c>
+      <c r="I16" t="s">
+        <v>449</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>172</v>
       </c>
@@ -2251,8 +2590,18 @@
       <c r="C17" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v>Arizona</v>
+      </c>
+      <c r="I17" t="s">
+        <v>450</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>351</v>
       </c>
@@ -2262,8 +2611,18 @@
       <c r="C18" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v>Arizona</v>
+      </c>
+      <c r="I18" t="s">
+        <v>451</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>104</v>
       </c>
@@ -2273,8 +2632,18 @@
       <c r="C19" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v>California</v>
+      </c>
+      <c r="I19" t="s">
+        <v>452</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>184</v>
       </c>
@@ -2284,8 +2653,18 @@
       <c r="C20" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v>California</v>
+      </c>
+      <c r="I20" t="s">
+        <v>453</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>111</v>
       </c>
@@ -2295,8 +2674,18 @@
       <c r="C21" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" t="str">
+        <f t="shared" si="0"/>
+        <v>California</v>
+      </c>
+      <c r="I21" t="s">
+        <v>454</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>350</v>
       </c>
@@ -2306,8 +2695,18 @@
       <c r="C22" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v>California</v>
+      </c>
+      <c r="I22" t="s">
+        <v>456</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>151</v>
       </c>
@@ -2317,8 +2716,18 @@
       <c r="C23" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" t="str">
+        <f t="shared" si="0"/>
+        <v>California</v>
+      </c>
+      <c r="I23" t="s">
+        <v>457</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>298</v>
       </c>
@@ -2328,8 +2737,18 @@
       <c r="C24" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" t="str">
+        <f t="shared" si="0"/>
+        <v>California</v>
+      </c>
+      <c r="I24" t="s">
+        <v>458</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>296</v>
       </c>
@@ -2339,8 +2758,18 @@
       <c r="C25" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v>California</v>
+      </c>
+      <c r="I25" t="s">
+        <v>459</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>224</v>
       </c>
@@ -2350,8 +2779,18 @@
       <c r="C26" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v>California</v>
+      </c>
+      <c r="I26" t="s">
+        <v>460</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>331</v>
       </c>
@@ -2361,8 +2800,18 @@
       <c r="C27" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" t="str">
+        <f t="shared" si="0"/>
+        <v>California</v>
+      </c>
+      <c r="I27" t="s">
+        <v>461</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>346</v>
       </c>
@@ -2372,8 +2821,18 @@
       <c r="C28" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" t="str">
+        <f t="shared" si="0"/>
+        <v>California</v>
+      </c>
+      <c r="I28" t="s">
+        <v>462</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>197</v>
       </c>
@@ -2383,8 +2842,18 @@
       <c r="C29" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29" t="str">
+        <f t="shared" si="0"/>
+        <v>Colorado</v>
+      </c>
+      <c r="I29" t="s">
+        <v>463</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>202</v>
       </c>
@@ -2394,8 +2863,18 @@
       <c r="C30" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30" t="str">
+        <f t="shared" si="0"/>
+        <v>Colorado</v>
+      </c>
+      <c r="I30" t="s">
+        <v>464</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>313</v>
       </c>
@@ -2405,8 +2884,18 @@
       <c r="C31" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31" t="str">
+        <f t="shared" si="0"/>
+        <v>Colorado</v>
+      </c>
+      <c r="I31" t="s">
+        <v>466</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>164</v>
       </c>
@@ -2416,8 +2905,18 @@
       <c r="C32" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32" t="str">
+        <f t="shared" si="0"/>
+        <v>Delaware</v>
+      </c>
+      <c r="I32" t="s">
+        <v>467</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>243</v>
       </c>
@@ -2427,8 +2926,18 @@
       <c r="C33" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33" t="str">
+        <f t="shared" si="0"/>
+        <v>Florida</v>
+      </c>
+      <c r="I33" t="s">
+        <v>468</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>126</v>
       </c>
@@ -2438,8 +2947,18 @@
       <c r="C34" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34" t="str">
+        <f t="shared" si="0"/>
+        <v>Florida</v>
+      </c>
+      <c r="I34" t="s">
+        <v>469</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>284</v>
       </c>
@@ -2449,8 +2968,18 @@
       <c r="C35" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35" t="str">
+        <f t="shared" si="0"/>
+        <v>Florida</v>
+      </c>
+      <c r="I35" t="s">
+        <v>470</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>95</v>
       </c>
@@ -2460,8 +2989,18 @@
       <c r="C36" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36" t="str">
+        <f t="shared" si="0"/>
+        <v>Florida</v>
+      </c>
+      <c r="I36" t="s">
+        <v>471</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>182</v>
       </c>
@@ -2471,8 +3010,18 @@
       <c r="C37" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37" t="str">
+        <f t="shared" si="0"/>
+        <v>Florida</v>
+      </c>
+      <c r="I37" t="s">
+        <v>472</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>336</v>
       </c>
@@ -2482,8 +3031,18 @@
       <c r="C38" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38" t="str">
+        <f t="shared" si="0"/>
+        <v>Florida</v>
+      </c>
+      <c r="I38" t="s">
+        <v>473</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>333</v>
       </c>
@@ -2493,8 +3052,18 @@
       <c r="C39" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39" t="str">
+        <f t="shared" si="0"/>
+        <v>Florida</v>
+      </c>
+      <c r="I39" t="s">
+        <v>474</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>191</v>
       </c>
@@ -2504,8 +3073,18 @@
       <c r="C40" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D40" t="str">
+        <f t="shared" si="0"/>
+        <v>Georgia</v>
+      </c>
+      <c r="I40" t="s">
+        <v>475</v>
+      </c>
+      <c r="J40" s="2" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>344</v>
       </c>
@@ -2515,8 +3094,18 @@
       <c r="C41" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41" t="str">
+        <f t="shared" si="0"/>
+        <v>Georgia</v>
+      </c>
+      <c r="I41" t="s">
+        <v>477</v>
+      </c>
+      <c r="J41" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>245</v>
       </c>
@@ -2526,8 +3115,18 @@
       <c r="C42" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42" t="str">
+        <f t="shared" si="0"/>
+        <v>Georgia</v>
+      </c>
+      <c r="I42" t="s">
+        <v>478</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>218</v>
       </c>
@@ -2537,8 +3136,18 @@
       <c r="C43" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D43" t="str">
+        <f t="shared" si="0"/>
+        <v>Hawaii</v>
+      </c>
+      <c r="I43" t="s">
+        <v>479</v>
+      </c>
+      <c r="J43" s="2" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>220</v>
       </c>
@@ -2548,8 +3157,18 @@
       <c r="C44" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44" t="str">
+        <f t="shared" si="0"/>
+        <v>Hawaii</v>
+      </c>
+      <c r="I44" t="s">
+        <v>480</v>
+      </c>
+      <c r="J44" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>222</v>
       </c>
@@ -2559,8 +3178,18 @@
       <c r="C45" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D45" t="str">
+        <f t="shared" si="0"/>
+        <v>Hawaii</v>
+      </c>
+      <c r="I45" t="s">
+        <v>481</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>228</v>
       </c>
@@ -2570,8 +3199,18 @@
       <c r="C46" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D46" t="str">
+        <f t="shared" si="0"/>
+        <v>Hawaii</v>
+      </c>
+      <c r="I46" t="s">
+        <v>482</v>
+      </c>
+      <c r="J46" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>162</v>
       </c>
@@ -2581,8 +3220,18 @@
       <c r="C47" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D47" t="str">
+        <f t="shared" si="0"/>
+        <v>Iowa</v>
+      </c>
+      <c r="I47" t="s">
+        <v>483</v>
+      </c>
+      <c r="J47" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>168</v>
       </c>
@@ -2592,8 +3241,18 @@
       <c r="C48" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D48" t="str">
+        <f t="shared" si="0"/>
+        <v>Iowa</v>
+      </c>
+      <c r="I48" t="s">
+        <v>484</v>
+      </c>
+      <c r="J48" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>133</v>
       </c>
@@ -2603,8 +3262,18 @@
       <c r="C49" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D49" t="str">
+        <f t="shared" si="0"/>
+        <v>Idaho</v>
+      </c>
+      <c r="I49" t="s">
+        <v>485</v>
+      </c>
+      <c r="J49" s="2" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>323</v>
       </c>
@@ -2614,8 +3283,18 @@
       <c r="C50" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D50" t="str">
+        <f t="shared" si="0"/>
+        <v>Idaho</v>
+      </c>
+      <c r="I50" t="s">
+        <v>486</v>
+      </c>
+      <c r="J50" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>235</v>
       </c>
@@ -2625,8 +3304,18 @@
       <c r="C51" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D51" t="str">
+        <f t="shared" si="0"/>
+        <v>Illinois</v>
+      </c>
+      <c r="I51" t="s">
+        <v>487</v>
+      </c>
+      <c r="J51" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>262</v>
       </c>
@@ -2636,8 +3325,12 @@
       <c r="C52" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D52" t="str">
+        <f t="shared" si="0"/>
+        <v>Illinois</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>237</v>
       </c>
@@ -2647,8 +3340,12 @@
       <c r="C53" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D53" t="str">
+        <f t="shared" si="0"/>
+        <v>Indiana</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>242</v>
       </c>
@@ -2658,8 +3355,12 @@
       <c r="C54" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D54" t="str">
+        <f t="shared" si="0"/>
+        <v>Indiana</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>152</v>
       </c>
@@ -2669,8 +3370,12 @@
       <c r="C55" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D55" t="str">
+        <f t="shared" si="0"/>
+        <v>Kansas</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>204</v>
       </c>
@@ -2680,8 +3385,12 @@
       <c r="C56" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D56" t="str">
+        <f t="shared" si="0"/>
+        <v>Kansas</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>339</v>
       </c>
@@ -2691,8 +3400,12 @@
       <c r="C57" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D57" t="str">
+        <f t="shared" si="0"/>
+        <v>Kansas</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>229</v>
       </c>
@@ -2702,8 +3415,12 @@
       <c r="C58" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D58" t="str">
+        <f t="shared" si="0"/>
+        <v>Kansas</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>225</v>
       </c>
@@ -2713,8 +3430,12 @@
       <c r="C59" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D59" t="str">
+        <f t="shared" si="0"/>
+        <v>Kentucky</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>247</v>
       </c>
@@ -2724,8 +3445,12 @@
       <c r="C60" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D60" t="str">
+        <f t="shared" si="0"/>
+        <v>Kentucky</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>270</v>
       </c>
@@ -2735,8 +3460,12 @@
       <c r="C61" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D61" t="str">
+        <f t="shared" si="0"/>
+        <v>Kentucky</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>307</v>
       </c>
@@ -2746,8 +3475,12 @@
       <c r="C62" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D62" t="str">
+        <f t="shared" si="0"/>
+        <v>Kentucky</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>312</v>
       </c>
@@ -2757,8 +3490,12 @@
       <c r="C63" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D63" t="str">
+        <f t="shared" si="0"/>
+        <v>Louisiana</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>253</v>
       </c>
@@ -2768,8 +3505,12 @@
       <c r="C64" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D64" t="str">
+        <f t="shared" si="0"/>
+        <v>Louisiana</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>256</v>
       </c>
@@ -2779,8 +3520,12 @@
       <c r="C65" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D65" t="str">
+        <f t="shared" si="0"/>
+        <v>Louisiana</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>327</v>
       </c>
@@ -2790,8 +3535,12 @@
       <c r="C66" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D66" t="str">
+        <f t="shared" ref="D66:D129" si="1">INDEX(I$2:I$51,MATCH(C66,J$2:J$51,0))</f>
+        <v>Louisiana</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>120</v>
       </c>
@@ -2801,8 +3550,12 @@
       <c r="C67" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D67" t="str">
+        <f t="shared" si="1"/>
+        <v>Massachusetts</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>131</v>
       </c>
@@ -2812,8 +3565,12 @@
       <c r="C68" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D68" t="str">
+        <f t="shared" si="1"/>
+        <v>Maine</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>214</v>
       </c>
@@ -2823,8 +3580,12 @@
       <c r="C69" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D69" t="str">
+        <f t="shared" si="1"/>
+        <v>Maine</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>167</v>
       </c>
@@ -2834,8 +3595,12 @@
       <c r="C70" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D70" t="str">
+        <f t="shared" si="1"/>
+        <v>Michigan</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>98</v>
       </c>
@@ -2845,8 +3610,12 @@
       <c r="C71" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D71" t="str">
+        <f t="shared" si="1"/>
+        <v>Michigan</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>209</v>
       </c>
@@ -2856,8 +3625,12 @@
       <c r="C72" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D72" t="str">
+        <f t="shared" si="1"/>
+        <v>Michigan</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>289</v>
       </c>
@@ -2867,8 +3640,12 @@
       <c r="C73" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D73" t="str">
+        <f t="shared" si="1"/>
+        <v>Michigan</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>159</v>
       </c>
@@ -2878,8 +3655,12 @@
       <c r="C74" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D74" t="str">
+        <f t="shared" si="1"/>
+        <v>Minnesota</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>288</v>
       </c>
@@ -2889,8 +3670,12 @@
       <c r="C75" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D75" t="str">
+        <f t="shared" si="1"/>
+        <v>Minnesota</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>170</v>
       </c>
@@ -2900,8 +3685,12 @@
       <c r="C76" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D76" t="str">
+        <f t="shared" si="1"/>
+        <v>Missouri</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>325</v>
       </c>
@@ -2911,8 +3700,12 @@
       <c r="C77" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D77" t="str">
+        <f t="shared" si="1"/>
+        <v>Missouri</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>266</v>
       </c>
@@ -2922,8 +3715,12 @@
       <c r="C78" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D78" t="str">
+        <f t="shared" si="1"/>
+        <v>Missouri</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>156</v>
       </c>
@@ -2933,8 +3730,12 @@
       <c r="C79" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D79" t="str">
+        <f t="shared" si="1"/>
+        <v>Mississippi</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>212</v>
       </c>
@@ -2944,8 +3745,12 @@
       <c r="C80" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D80" t="str">
+        <f t="shared" si="1"/>
+        <v>Mississippi</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>115</v>
       </c>
@@ -2955,8 +3760,12 @@
       <c r="C81" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D81" t="str">
+        <f t="shared" si="1"/>
+        <v>Montana</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>200</v>
       </c>
@@ -2966,8 +3775,12 @@
       <c r="C82" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D82" t="str">
+        <f t="shared" si="1"/>
+        <v>Montana</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>334</v>
       </c>
@@ -2977,8 +3790,12 @@
       <c r="C83" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D83" t="str">
+        <f t="shared" si="1"/>
+        <v>Montana</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>293</v>
       </c>
@@ -2988,8 +3805,12 @@
       <c r="C84" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D84" t="str">
+        <f t="shared" si="1"/>
+        <v>Montana</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>282</v>
       </c>
@@ -2999,8 +3820,12 @@
       <c r="C85" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D85" t="str">
+        <f t="shared" si="1"/>
+        <v>North Carolina</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>315</v>
       </c>
@@ -3010,8 +3835,12 @@
       <c r="C86" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D86" t="str">
+        <f t="shared" si="1"/>
+        <v>North Carolina</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>267</v>
       </c>
@@ -3021,8 +3850,12 @@
       <c r="C87" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D87" t="str">
+        <f t="shared" si="1"/>
+        <v>North Carolina</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>112</v>
       </c>
@@ -3032,8 +3865,12 @@
       <c r="C88" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D88" t="str">
+        <f t="shared" si="1"/>
+        <v>North Dakota</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>297</v>
       </c>
@@ -3043,8 +3880,12 @@
       <c r="C89" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D89" t="str">
+        <f t="shared" si="1"/>
+        <v>North Dakota</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>280</v>
       </c>
@@ -3054,8 +3895,12 @@
       <c r="C90" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D90" t="str">
+        <f t="shared" si="1"/>
+        <v>North Dakota</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>343</v>
       </c>
@@ -3065,8 +3910,12 @@
       <c r="C91" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D91" t="str">
+        <f t="shared" si="1"/>
+        <v>Nebraska</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>259</v>
       </c>
@@ -3076,8 +3925,12 @@
       <c r="C92" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D92" t="str">
+        <f t="shared" si="1"/>
+        <v>Nebraska</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>301</v>
       </c>
@@ -3087,8 +3940,12 @@
       <c r="C93" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D93" t="str">
+        <f t="shared" si="1"/>
+        <v>Nebraska</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>158</v>
       </c>
@@ -3098,8 +3955,12 @@
       <c r="C94" t="s">
         <v>406</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D94" t="str">
+        <f t="shared" si="1"/>
+        <v>New Jersey</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>84</v>
       </c>
@@ -3109,8 +3970,12 @@
       <c r="C95" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D95" t="str">
+        <f t="shared" si="1"/>
+        <v>New Mexico</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>190</v>
       </c>
@@ -3120,8 +3985,12 @@
       <c r="C96" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D96" t="str">
+        <f t="shared" si="1"/>
+        <v>New Mexico</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>215</v>
       </c>
@@ -3131,8 +4000,12 @@
       <c r="C97" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D97" t="str">
+        <f t="shared" si="1"/>
+        <v>New Mexico</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>264</v>
       </c>
@@ -3142,8 +4015,12 @@
       <c r="C98" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D98" t="str">
+        <f t="shared" si="1"/>
+        <v>Nevada</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>179</v>
       </c>
@@ -3153,8 +4030,12 @@
       <c r="C99" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D99" t="str">
+        <f t="shared" si="1"/>
+        <v>Nevada</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>318</v>
       </c>
@@ -3164,8 +4045,12 @@
       <c r="C100" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D100" t="str">
+        <f t="shared" si="1"/>
+        <v>Nevada</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>175</v>
       </c>
@@ -3175,8 +4060,12 @@
       <c r="C101" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D101" t="str">
+        <f t="shared" si="1"/>
+        <v>New York</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>107</v>
       </c>
@@ -3186,8 +4075,12 @@
       <c r="C102" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D102" t="str">
+        <f t="shared" si="1"/>
+        <v>New York</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>124</v>
       </c>
@@ -3197,8 +4090,12 @@
       <c r="C103" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D103" t="str">
+        <f t="shared" si="1"/>
+        <v>New York</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>340</v>
       </c>
@@ -3208,8 +4105,12 @@
       <c r="C104" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D104" t="str">
+        <f t="shared" si="1"/>
+        <v>New York</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>304</v>
       </c>
@@ -3219,8 +4120,12 @@
       <c r="C105" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D105" t="str">
+        <f t="shared" si="1"/>
+        <v>New York</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>138</v>
       </c>
@@ -3230,8 +4135,12 @@
       <c r="C106" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D106" t="str">
+        <f t="shared" si="1"/>
+        <v>Ohio</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>234</v>
       </c>
@@ -3241,8 +4150,12 @@
       <c r="C107" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D107" t="str">
+        <f t="shared" si="1"/>
+        <v>Ohio</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>187</v>
       </c>
@@ -3252,8 +4165,12 @@
       <c r="C108" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D108" t="str">
+        <f t="shared" si="1"/>
+        <v>Oklahoma</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>338</v>
       </c>
@@ -3263,8 +4180,12 @@
       <c r="C109" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D109" t="str">
+        <f t="shared" si="1"/>
+        <v>Oklahoma</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>240</v>
       </c>
@@ -3274,8 +4195,12 @@
       <c r="C110" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D110" t="str">
+        <f t="shared" si="1"/>
+        <v>Oklahoma</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>348</v>
       </c>
@@ -3285,8 +4210,12 @@
       <c r="C111" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D111" t="str">
+        <f t="shared" si="1"/>
+        <v>Oklahoma</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>277</v>
       </c>
@@ -3296,8 +4225,12 @@
       <c r="C112" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D112" t="str">
+        <f t="shared" si="1"/>
+        <v>Oregon</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>310</v>
       </c>
@@ -3307,8 +4240,12 @@
       <c r="C113" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D113" t="str">
+        <f t="shared" si="1"/>
+        <v>Oregon</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>321</v>
       </c>
@@ -3318,8 +4255,12 @@
       <c r="C114" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D114" t="str">
+        <f t="shared" si="1"/>
+        <v>Oregon</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>309</v>
       </c>
@@ -3329,8 +4270,12 @@
       <c r="C115" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D115" t="str">
+        <f t="shared" si="1"/>
+        <v>Pennsylvania</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>136</v>
       </c>
@@ -3340,8 +4285,12 @@
       <c r="C116" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D116" t="str">
+        <f t="shared" si="1"/>
+        <v>Pennsylvania</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>249</v>
       </c>
@@ -3351,8 +4300,12 @@
       <c r="C117" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D117" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>141</v>
       </c>
@@ -3362,8 +4315,12 @@
       <c r="C118" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D118" t="str">
+        <f t="shared" si="1"/>
+        <v>South Carolina</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>128</v>
       </c>
@@ -3373,8 +4330,12 @@
       <c r="C119" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D119" t="str">
+        <f t="shared" si="1"/>
+        <v>South Carolina</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>211</v>
       </c>
@@ -3384,8 +4345,12 @@
       <c r="C120" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D120" t="str">
+        <f t="shared" si="1"/>
+        <v>South Carolina</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>81</v>
       </c>
@@ -3395,8 +4360,12 @@
       <c r="C121" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D121" t="str">
+        <f t="shared" si="1"/>
+        <v>South Dakota</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>341</v>
       </c>
@@ -3406,8 +4375,12 @@
       <c r="C122" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D122" t="str">
+        <f t="shared" si="1"/>
+        <v>South Dakota</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>193</v>
       </c>
@@ -3417,8 +4390,12 @@
       <c r="C123" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D123" t="str">
+        <f t="shared" si="1"/>
+        <v>South Dakota</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>291</v>
       </c>
@@ -3428,8 +4405,12 @@
       <c r="C124" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D124" t="str">
+        <f t="shared" si="1"/>
+        <v>Tennessee</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>300</v>
       </c>
@@ -3439,8 +4420,12 @@
       <c r="C125" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D125" t="str">
+        <f t="shared" si="1"/>
+        <v>Tennessee</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>303</v>
       </c>
@@ -3450,8 +4435,12 @@
       <c r="C126" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D126" t="str">
+        <f t="shared" si="1"/>
+        <v>Tennessee</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>92</v>
       </c>
@@ -3461,8 +4450,12 @@
       <c r="C127" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D127" t="str">
+        <f t="shared" si="1"/>
+        <v>Texas</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>183</v>
       </c>
@@ -3472,8 +4465,12 @@
       <c r="C128" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D128" t="str">
+        <f t="shared" si="1"/>
+        <v>Texas</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>122</v>
       </c>
@@ -3483,8 +4480,12 @@
       <c r="C129" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D129" t="str">
+        <f t="shared" si="1"/>
+        <v>Texas</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>208</v>
       </c>
@@ -3494,8 +4495,12 @@
       <c r="C130" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D130" t="str">
+        <f t="shared" ref="D130:D154" si="2">INDEX(I$2:I$51,MATCH(C130,J$2:J$51,0))</f>
+        <v>Texas</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>143</v>
       </c>
@@ -3505,8 +4510,12 @@
       <c r="C131" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D131" t="str">
+        <f t="shared" si="2"/>
+        <v>Texas</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>199</v>
       </c>
@@ -3516,8 +4525,12 @@
       <c r="C132" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D132" t="str">
+        <f t="shared" si="2"/>
+        <v>Texas</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>169</v>
       </c>
@@ -3527,8 +4540,12 @@
       <c r="C133" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D133" t="str">
+        <f t="shared" si="2"/>
+        <v>Texas</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>177</v>
       </c>
@@ -3538,8 +4555,12 @@
       <c r="C134" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D134" t="str">
+        <f t="shared" si="2"/>
+        <v>Texas</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>217</v>
       </c>
@@ -3549,8 +4570,12 @@
       <c r="C135" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D135" t="str">
+        <f t="shared" si="2"/>
+        <v>Texas</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>155</v>
       </c>
@@ -3560,8 +4585,12 @@
       <c r="C136" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D136" t="str">
+        <f t="shared" si="2"/>
+        <v>Texas</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>251</v>
       </c>
@@ -3571,8 +4600,12 @@
       <c r="C137" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D137" t="str">
+        <f t="shared" si="2"/>
+        <v>Texas</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>275</v>
       </c>
@@ -3582,8 +4615,12 @@
       <c r="C138" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D138" t="str">
+        <f t="shared" si="2"/>
+        <v>Texas</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>329</v>
       </c>
@@ -3593,8 +4630,12 @@
       <c r="C139" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D139" t="str">
+        <f t="shared" si="2"/>
+        <v>Texas</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>231</v>
       </c>
@@ -3604,8 +4645,12 @@
       <c r="C140" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D140" t="str">
+        <f t="shared" si="2"/>
+        <v>Utah</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>294</v>
       </c>
@@ -3615,8 +4660,12 @@
       <c r="C141" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D141" t="str">
+        <f t="shared" si="2"/>
+        <v>Utah</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>186</v>
       </c>
@@ -3626,8 +4675,12 @@
       <c r="C142" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D142" t="str">
+        <f t="shared" si="2"/>
+        <v>Virginia</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>271</v>
       </c>
@@ -3637,8 +4690,12 @@
       <c r="C143" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D143" t="str">
+        <f t="shared" si="2"/>
+        <v>Virginia</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>90</v>
       </c>
@@ -3648,8 +4705,12 @@
       <c r="C144" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D144" t="str">
+        <f t="shared" si="2"/>
+        <v>Virginia</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>145</v>
       </c>
@@ -3659,8 +4720,12 @@
       <c r="C145" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D145" t="str">
+        <f t="shared" si="2"/>
+        <v>Vermont</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>257</v>
       </c>
@@ -3670,8 +4735,12 @@
       <c r="C146" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D146" t="str">
+        <f t="shared" si="2"/>
+        <v>Washington</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>102</v>
       </c>
@@ -3681,8 +4750,12 @@
       <c r="C147" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D147" t="str">
+        <f t="shared" si="2"/>
+        <v>Washington</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>305</v>
       </c>
@@ -3692,8 +4765,12 @@
       <c r="C148" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D148" t="str">
+        <f t="shared" si="2"/>
+        <v>Washington</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>206</v>
       </c>
@@ -3703,8 +4780,12 @@
       <c r="C149" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D149" t="str">
+        <f t="shared" si="2"/>
+        <v>Wisconsin</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>100</v>
       </c>
@@ -3714,8 +4795,12 @@
       <c r="C150" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D150" t="str">
+        <f t="shared" si="2"/>
+        <v>Wisconsin</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>283</v>
       </c>
@@ -3725,8 +4810,12 @@
       <c r="C151" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D151" t="str">
+        <f t="shared" si="2"/>
+        <v>Wisconsin</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>319</v>
       </c>
@@ -3736,8 +4825,12 @@
       <c r="C152" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D152" t="str">
+        <f t="shared" si="2"/>
+        <v>West Virginia</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>148</v>
       </c>
@@ -3747,8 +4840,12 @@
       <c r="C153" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D153" t="str">
+        <f t="shared" si="2"/>
+        <v>Wyoming</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>316</v>
       </c>
@@ -3757,6 +4854,10 @@
       </c>
       <c r="C154" t="s">
         <v>150</v>
+      </c>
+      <c r="D154" t="str">
+        <f t="shared" si="2"/>
+        <v>Wyoming</v>
       </c>
     </row>
   </sheetData>

</xml_diff>